<commit_message>
maf formatting to string
</commit_message>
<xml_diff>
--- a/docs/metabobank/maf_excel/MetaboBank_maf_MS.xlsx
+++ b/docs/metabobank/maf_excel/MetaboBank_maf_MS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C936F2D-886E-4360-8459-E31FB8118D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10536"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="12" r:id="rId1"/>
@@ -151,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -229,15 +230,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -276,9 +275,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,9 +315,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -353,7 +352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,7 +560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
@@ -589,72 +588,68 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="6">
-        <v>44917</v>
+      <c r="B10" s="3">
+        <v>45363</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>44509</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>44645</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>44763</v>
       </c>
     </row>
@@ -662,12 +657,12 @@
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>44917</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
+      <c r="B17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -682,127 +677,127 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="57.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="61.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="28.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="34" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="38" width="40.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="41" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="27.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="50" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="53" width="46.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="56" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="59" width="30.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="62" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="68" width="33.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="71" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="75" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="79" width="27.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="83" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="84" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="39.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="57.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="61.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="28.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="30.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="34.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="38" width="40.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="28.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="45" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="50" width="25.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="46.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="28.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="59" width="30.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="62" width="31.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="68" width="33.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="71" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="75" width="27.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="79" width="27.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="83" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>